<commit_message>
reportes excel asignacion/transferencia/devolucion concluidos
</commit_message>
<xml_diff>
--- a/reportes/Asignacion.xlsx
+++ b/reportes/Asignacion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>FORMULARIO DE ASIGNACION DE ACTIVOS FIJOS</t>
   </si>
@@ -71,18 +71,6 @@
     <t>OBSERVACIONES</t>
   </si>
   <si>
-    <t>RESPONSABLE</t>
-  </si>
-  <si>
-    <t>RECIBI CONFORME</t>
-  </si>
-  <si>
-    <t>* CUSTODIO</t>
-  </si>
-  <si>
-    <t>* Esta casilla sera firmada por personal que trabaja en la empresa pero no figura en las planillas de BOA</t>
-  </si>
-  <si>
     <t>DENOMINACIÓN</t>
   </si>
 </sst>
@@ -90,7 +78,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,14 +117,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,6 +150,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -177,16 +168,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <bottom style="thin">
         <color indexed="64"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -197,14 +181,16 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -217,19 +203,9 @@
     <xf numFmtId="12" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -237,51 +213,85 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H22"/>
+  <dimension ref="B1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:D15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,275 +660,956 @@
     <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="30" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
       <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="31" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H4" s="6"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="31" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="11"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>19</v>
+      <c r="D10" s="6" t="s">
+        <v>15</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="29"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-    </row>
-    <row r="12" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-    </row>
-    <row r="13" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+    </row>
+    <row r="13" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="23"/>
       <c r="C14" s="23"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="22"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="12"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="35"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="25"/>
+      <c r="C56" s="25"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="35"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="25"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="35"/>
+      <c r="H57" s="35"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="35"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="35"/>
+      <c r="H59" s="35"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="35"/>
+      <c r="H60" s="35"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="25"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="35"/>
+      <c r="H61" s="35"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="27"/>
+      <c r="G62" s="35"/>
+      <c r="H62" s="35"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="35"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="35"/>
+      <c r="H64" s="35"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="35"/>
+      <c r="H65" s="35"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="35"/>
+      <c r="H66" s="35"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="34"/>
+      <c r="F67" s="27"/>
+      <c r="G67" s="35"/>
+      <c r="H67" s="35"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="25"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="34"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="35"/>
+      <c r="H68" s="35"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="25"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="35"/>
+      <c r="H69" s="35"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="27"/>
+      <c r="G70" s="35"/>
+      <c r="H70" s="35"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="34"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="35"/>
+      <c r="H71" s="35"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="35"/>
+      <c r="H72" s="35"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="34"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="35"/>
+      <c r="H73" s="35"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="25"/>
+      <c r="C74" s="25"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="27"/>
+      <c r="G74" s="35"/>
+      <c r="H74" s="35"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="25"/>
+      <c r="C75" s="25"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="27"/>
+      <c r="G75" s="35"/>
+      <c r="H75" s="35"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="34"/>
+      <c r="F76" s="27"/>
+      <c r="G76" s="35"/>
+      <c r="H76" s="35"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="25"/>
+      <c r="C77" s="25"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="34"/>
+      <c r="F77" s="27"/>
+      <c r="G77" s="35"/>
+      <c r="H77" s="35"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="25"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="34"/>
+      <c r="F78" s="27"/>
+      <c r="G78" s="35"/>
+      <c r="H78" s="35"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="25"/>
+      <c r="C79" s="25"/>
+      <c r="D79" s="34"/>
+      <c r="E79" s="34"/>
+      <c r="F79" s="27"/>
+      <c r="G79" s="35"/>
+      <c r="H79" s="35"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="25"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="27"/>
+      <c r="G80" s="35"/>
+      <c r="H80" s="35"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="25"/>
+      <c r="C81" s="25"/>
+      <c r="D81" s="34"/>
+      <c r="E81" s="34"/>
+      <c r="F81" s="27"/>
+      <c r="G81" s="35"/>
+      <c r="H81" s="35"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="25"/>
+      <c r="C82" s="25"/>
+      <c r="D82" s="34"/>
+      <c r="E82" s="34"/>
+      <c r="F82" s="27"/>
+      <c r="G82" s="35"/>
+      <c r="H82" s="35"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="25"/>
+      <c r="C83" s="25"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="34"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="35"/>
+      <c r="H83" s="35"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="25"/>
+      <c r="C84" s="25"/>
+      <c r="D84" s="34"/>
+      <c r="E84" s="34"/>
+      <c r="F84" s="27"/>
+      <c r="G84" s="35"/>
+      <c r="H84" s="35"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="25"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="34"/>
+      <c r="E85" s="34"/>
+      <c r="F85" s="27"/>
+      <c r="G85" s="35"/>
+      <c r="H85" s="35"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="25"/>
+      <c r="C86" s="25"/>
+      <c r="D86" s="34"/>
+      <c r="E86" s="34"/>
+      <c r="F86" s="27"/>
+      <c r="G86" s="35"/>
+      <c r="H86" s="35"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="25"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="34"/>
+      <c r="E87" s="34"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="35"/>
+      <c r="H87" s="35"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="25"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="34"/>
+      <c r="E88" s="34"/>
+      <c r="F88" s="27"/>
+      <c r="G88" s="35"/>
+      <c r="H88" s="35"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="25"/>
+      <c r="C89" s="25"/>
+      <c r="D89" s="34"/>
+      <c r="E89" s="34"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="35"/>
+      <c r="H89" s="35"/>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="25"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="34"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="27"/>
+      <c r="G90" s="35"/>
+      <c r="H90" s="35"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="25"/>
+      <c r="C91" s="25"/>
+      <c r="D91" s="34"/>
+      <c r="E91" s="34"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="35"/>
+      <c r="H91" s="35"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="25"/>
+      <c r="C92" s="25"/>
+      <c r="D92" s="34"/>
+      <c r="E92" s="34"/>
+      <c r="F92" s="27"/>
+      <c r="G92" s="35"/>
+      <c r="H92" s="35"/>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="25"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="34"/>
+      <c r="E93" s="34"/>
+      <c r="F93" s="27"/>
+      <c r="G93" s="35"/>
+      <c r="H93" s="35"/>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="25"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="34"/>
+      <c r="E94" s="34"/>
+      <c r="F94" s="27"/>
+      <c r="G94" s="35"/>
+      <c r="H94" s="35"/>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="25"/>
+      <c r="C95" s="25"/>
+      <c r="D95" s="34"/>
+      <c r="E95" s="34"/>
+      <c r="F95" s="27"/>
+      <c r="G95" s="35"/>
+      <c r="H95" s="35"/>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="25"/>
+      <c r="C96" s="25"/>
+      <c r="D96" s="34"/>
+      <c r="E96" s="34"/>
+      <c r="F96" s="27"/>
+      <c r="G96" s="35"/>
+      <c r="H96" s="35"/>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="25"/>
+      <c r="C97" s="25"/>
+      <c r="D97" s="34"/>
+      <c r="E97" s="34"/>
+      <c r="F97" s="27"/>
+      <c r="G97" s="35"/>
+      <c r="H97" s="35"/>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="25"/>
+      <c r="C98" s="25"/>
+      <c r="D98" s="34"/>
+      <c r="E98" s="34"/>
+      <c r="F98" s="27"/>
+      <c r="G98" s="35"/>
+      <c r="H98" s="35"/>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="25"/>
+      <c r="C99" s="25"/>
+      <c r="D99" s="34"/>
+      <c r="E99" s="34"/>
+      <c r="F99" s="27"/>
+      <c r="G99" s="35"/>
+      <c r="H99" s="35"/>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="25"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="34"/>
+      <c r="E100" s="34"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="35"/>
+      <c r="H100" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="13">
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H8"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="B9:H9"/>
     <mergeCell ref="B1:C3"/>
     <mergeCell ref="D1:F2"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H8"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>

</xml_diff>